<commit_message>
Code permettant de récupérer les Tweets OK
</commit_message>
<xml_diff>
--- a/NomProjet.xlsx
+++ b/NomProjet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierrea\Documents\GitHub\Twitter-Elections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf56cabda597f9b3/Bureau/Formations/01_UTT/Cours/28_Babiga/Projet/Github_projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189B1846-9213-481B-8C85-2BAB2F713328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{189B1846-9213-481B-8C85-2BAB2F713328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD055F5D-81B7-4A98-9E2A-B8935FBC717F}"/>
   <bookViews>
-    <workbookView xWindow="-27630" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ElecTweets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elections letweetlatives </t>
+  </si>
+  <si>
+    <t>:p</t>
+  </si>
+  <si>
+    <t>Future is tweet</t>
+  </si>
+  <si>
+    <t>Jeu de mot avec "futuristic"… mais pas évident !</t>
   </si>
 </sst>
 </file>
@@ -345,20 +357,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>